<commit_message>
Improve missing guards + new missing file
</commit_message>
<xml_diff>
--- a/שבצ״ק.xlsx
+++ b/שבצ״ק.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybenichou/Desktop/meshavsek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51839A7-4435-F043-82A8-31BD54D4BBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F837AAAB-DA71-624E-BF8F-C3B053FB1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="שבצ״כ" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
   <si>
     <t>יום</t>
   </si>
@@ -40,26 +40,169 @@
     <t>פטרול</t>
   </si>
   <si>
-    <t>ו</t>
+    <t>כתת כוננות</t>
+  </si>
+  <si>
+    <t>שבת</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>שראל בלוך
+נתנאל שרעבי</t>
+  </si>
+  <si>
+    <t>דימטרי יוספוב
+סרגיי שבצוב</t>
+  </si>
+  <si>
+    <t>אור נצקנסקי
+עדן אסרף</t>
+  </si>
+  <si>
+    <t>6 תורני רס"פ - חדר</t>
+  </si>
+  <si>
+    <t>5 חדר</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>אבנר איזרבביץ'
+סרגיי לומיאנסקי</t>
+  </si>
+  <si>
+    <t>איתי כהן
+נריה כלפה</t>
+  </si>
+  <si>
+    <t>לוטם עטיה
+איתי סיני</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>דעאל כהן
+שגיא אריה</t>
+  </si>
+  <si>
+    <t>לואיס אברבוך
+אנזו גואטה</t>
+  </si>
+  <si>
+    <t>אנדי בנישו
+דוד סספורטס</t>
+  </si>
+  <si>
+    <t>11 חדר</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>מיכאל נפמן
+מאיר סדון</t>
+  </si>
+  <si>
+    <t>ארד רז
+יואל אודיז</t>
+  </si>
+  <si>
+    <t>ליאור אבו חמדה
+משה אייכנשטין</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>נדב קריספין
+יוסף רווה</t>
+  </si>
+  <si>
+    <t>עדן אסרף
+אסף זבולון</t>
+  </si>
+  <si>
+    <t>דורון לביא
+שמעון ספנייב</t>
+  </si>
+  <si>
+    <t>10 חדר</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>מרדוש דהאן
+אור נצקנסקי</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>אייל דבוש
+גיא פיאצה</t>
+  </si>
+  <si>
+    <t>א</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>01:00</t>
   </si>
   <si>
     <t>02:00</t>
   </si>
   <si>
-    <t>אבנר
-שגיא</t>
-  </si>
-  <si>
-    <t>דימה
-שבצוב</t>
-  </si>
-  <si>
-    <t>אור
-אסרף</t>
-  </si>
-  <si>
-    <t>לוטם
-סיני</t>
+    <t>דובר אלבז
+נריה כלפה</t>
+  </si>
+  <si>
+    <t>אלכסיי ברומברג
+סרגיי לומיאנסקי</t>
+  </si>
+  <si>
+    <t>יהונתן דימנטמן
+ירין מטמוני</t>
+  </si>
+  <si>
+    <t>אבנר איזרבביץ'
+עומרי דותן</t>
+  </si>
+  <si>
+    <t>9 חדר</t>
   </si>
   <si>
     <t>03:00</t>
@@ -71,195 +214,76 @@
     <t>05:00</t>
   </si>
   <si>
-    <t>אנזו
-שרעבי</t>
-  </si>
-  <si>
-    <t>דימנטמן
-מטמוני</t>
-  </si>
-  <si>
-    <t>דותן
-ליאור</t>
+    <t>איתי סיני
+לוטם עטיה</t>
+  </si>
+  <si>
+    <t>דעאל כהן
+אגומס מלדה</t>
+  </si>
+  <si>
+    <t>שגיא אריה
+איתי כהן</t>
   </si>
   <si>
     <t>06:00</t>
   </si>
   <si>
+    <t>7 תורני רס"פ - חדר</t>
+  </si>
+  <si>
     <t>07:00</t>
   </si>
   <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>אלכסיי
-לומיאנסקי</t>
-  </si>
-  <si>
-    <t>דעאל
-לואיס</t>
-  </si>
-  <si>
-    <t>אנדי
-דוד</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>כלפה
-שמעון</t>
-  </si>
-  <si>
-    <t>ארד
-יואל</t>
-  </si>
-  <si>
-    <t>נפמן
-סדון</t>
-  </si>
-  <si>
-    <t>12:00</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>מרדש
-משה</t>
-  </si>
-  <si>
-    <t>אסף
-דורון</t>
-  </si>
-  <si>
-    <t>קריספין
-רווה</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>דבוש
-פיאצה</t>
-  </si>
-  <si>
-    <t>שראל
-שרעבי</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>אבנר
-איתי כהן</t>
-  </si>
-  <si>
-    <t>21:00</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>דעאל
-לומיאנסקי</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>אנזו
-כלפה</t>
-  </si>
-  <si>
-    <t>שבת</t>
-  </si>
-  <si>
-    <t>00:00</t>
-  </si>
-  <si>
-    <t>01:00</t>
-  </si>
-  <si>
-    <t>אבנר
-לומיאנסקי</t>
-  </si>
-  <si>
-    <t>דעאל
-שגיא</t>
-  </si>
-  <si>
-    <t>ליאור
-משה</t>
-  </si>
-  <si>
-    <t>שגיא
-ליאור</t>
-  </si>
-  <si>
-    <t>לואיס
-שמעון</t>
+    <t>8 חדר</t>
+  </si>
+  <si>
+    <t>ליאור אבו חמדה
+אנזו גואטה</t>
+  </si>
+  <si>
+    <t>לואיס אברבוך
+יונתן יונג</t>
+  </si>
+  <si>
+    <t>משה אייכנשטין
+שמעון ספנייב</t>
+  </si>
+  <si>
+    <t>מרדוש דהאן
+עמיחי נעים</t>
+  </si>
+  <si>
+    <t>עומרי דותן
+אור נצקנסקי</t>
+  </si>
+  <si>
+    <t>אבנר איזרבביץ'
+מיכאל ניסנוב</t>
+  </si>
+  <si>
+    <t>6 חדר</t>
   </si>
   <si>
     <t>איתי כהן
-כלפה</t>
-  </si>
-  <si>
-    <t>לואיס
-אנזו</t>
-  </si>
-  <si>
-    <t xml:space="preserve">תורני רס"פ-
-  חדר 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> תורני רס"פ-
-  חדר 6</t>
-  </si>
-  <si>
-    <t>כתת כוננות</t>
-  </si>
-  <si>
-    <t>חדר 9</t>
-  </si>
-  <si>
-    <t>חדר 7</t>
-  </si>
-  <si>
-    <t>חדר 12</t>
-  </si>
-  <si>
-    <t>חדר 10</t>
-  </si>
-  <si>
-    <t>חדר 8</t>
-  </si>
-  <si>
-    <t>חדר 5</t>
-  </si>
-  <si>
-    <t>חדר 11</t>
+עמיחי נעים</t>
+  </si>
+  <si>
+    <t>ב</t>
+  </si>
+  <si>
+    <t>7 חדר</t>
+  </si>
+  <si>
+    <t>8 תורני רס"פ - חדר</t>
+  </si>
+  <si>
+    <t>עומרי דותן
+מיכאל ניסנוב</t>
+  </si>
+  <si>
+    <t>יואל אודיז
+ארד רז</t>
   </si>
 </sst>
 </file>
@@ -631,24 +655,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="3" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,628 +690,894 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G32" s="3"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="G38:G43"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="G20:G25"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F6:F21"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="F30:F43"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A43"/>
+  <mergeCells count="79">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A18:A41"/>
+    <mergeCell ref="A42:A61"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C10"/>
@@ -1303,6 +1592,68 @@
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="C38:C40"/>
     <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F44:F47"/>
+    <mergeCell ref="F48:F61"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="G26:G37"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="G50:G55"/>
+    <mergeCell ref="G56:G61"/>
+    <mergeCell ref="F2:F15"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F24:F39"/>
+    <mergeCell ref="F40:F43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>